<commit_message>
Co-authored-by: Alan Ye Yansong <neongasyy@users.noreply.github.com> Co-authored-by: Barry Ng <barryyng@users.noreply.github.com> Co-authored-by: Frizzante16 <Frizzante16@users.noreply.github.com> Co-authored-by: dragon21356 <dragon21356@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/OOPproj2002/src/pkg_camp/enquiries.xlsx
+++ b/OOPproj2002/src/pkg_camp/enquiries.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Camp Name</t>
   </si>
@@ -30,27 +30,6 @@
   </si>
   <si>
     <t>Reply</t>
-  </si>
-  <si>
-    <t>camp1</t>
-  </si>
-  <si>
-    <t>YCHERN</t>
-  </si>
-  <si>
-    <t>testing</t>
-  </si>
-  <si>
-    <t>omgitworks</t>
-  </si>
-  <si>
-    <t>CT113</t>
-  </si>
-  <si>
-    <t>CAMP_COMMITTEE_MEMBER</t>
-  </si>
-  <si>
-    <t>yeahitdoes</t>
   </si>
 </sst>
 </file>
@@ -95,7 +74,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -121,26 +100,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>12</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>